<commit_message>
complete map system redesign
</commit_message>
<xml_diff>
--- a/ZweiHander/Content/newDungeon1.xlsx
+++ b/ZweiHander/Content/newDungeon1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\Desktop\zwei-hander\ZweiHander\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{835E9363-DF1C-4EF7-A9A3-ABBB72A6C747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DE9A12-7DEC-422D-B7D8-EC1F704FC82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E1E3ECAE-D2E1-4D1B-AD4D-A86AE3EA36A1}"/>
+    <workbookView xWindow="17070" yWindow="0" windowWidth="11835" windowHeight="15585" xr2:uid="{E1E3ECAE-D2E1-4D1B-AD4D-A86AE3EA36A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="5">
   <si>
     <t>room.1</t>
   </si>
   <si>
     <t>b.1</t>
+  </si>
+  <si>
+    <t>b.1, b.3</t>
+  </si>
+  <si>
+    <t>b.1, b.10</t>
+  </si>
+  <si>
+    <t>b.1, e.1</t>
   </si>
 </sst>
 </file>
@@ -413,26 +422,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C65F5F-F2AE-4314-A9F0-0A607CBCF52B}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>